<commit_message>
Excel for Array - Practice
</commit_message>
<xml_diff>
--- a/09 - БДСУММ/Assignm13.xlsx
+++ b/09 - БДСУММ/Assignm13.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="9">
   <si>
     <t>Артикул</t>
   </si>
@@ -63,14 +63,14 @@
   <si>
     <t>Восток</t>
   </si>
+  <si>
+    <t>ФОРМУЛА  =БДСУММ(A1:D176;"Объем продаж";H1:K3)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₸_-;\-* #,##0.00\ _₸_-;_-* &quot;-&quot;??\ _₸_-;_-@_-"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,12 +90,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF2D2F31"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -136,9 +136,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -146,11 +145,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -465,7 +463,7 @@
   <dimension ref="A1:K176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,8 +472,7 @@
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="8.5546875" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="8" max="9" width="9.5546875" customWidth="1"/>
     <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -509,7 +506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -522,18 +519,16 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="str">
-        <f>A2</f>
-        <v>Север</v>
-      </c>
-      <c r="I2" s="4">
-        <f>B3</f>
+      <c r="H2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5">
         <v>234514</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -546,8 +541,12 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5">
+        <v>234514</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
@@ -564,6 +563,10 @@
       <c r="D4">
         <v>2</v>
       </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -578,10 +581,6 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="I5" s="5" t="e">
-        <f>DSUM(A1:D176,C:C,H1:K2)</f>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -596,6 +595,10 @@
       <c r="D6">
         <v>3</v>
       </c>
+      <c r="H6">
+        <f>DSUM(A1:D176,"Объем продаж",H1:K3)</f>
+        <v>2983</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -623,6 +626,9 @@
       </c>
       <c r="D8">
         <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>